<commit_message>
fixed some erros with headers
</commit_message>
<xml_diff>
--- a/data/xtd.xlsx
+++ b/data/xtd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbourim/Documents/Development/Github/dashboard_rev/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB1172D-818F-7449-8C29-4ACEA80F2B9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32ABB4B-CAE2-7F41-879E-D31E9D8F19E1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4380" yWindow="740" windowWidth="25020" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2303,7 +2303,9 @@
   </sheetPr>
   <dimension ref="A1:Y385"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>